<commit_message>
0108 道具bug fix all
</commit_message>
<xml_diff>
--- a/Mahtris 108/Assets/Document/Mahtris 108.xlsx
+++ b/Mahtris 108/Assets/Document/Mahtris 108.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dabbido\Desktop\Game Dev\GitHub\Mahtris-108\Mahtris 108\Assets\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7796A967-4B06-4931-BF64-462D72E70C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28D8D52-A72F-43F0-B5BA-A9DBC53542D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3181,7 +3181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3218,12 +3218,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3239,7 +3233,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3355,15 +3349,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3639,7 +3624,7 @@
   <dimension ref="A1:N67"/>
   <sheetViews>
     <sheetView topLeftCell="A31" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -5041,8 +5026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -5216,7 +5201,7 @@
       <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="37" t="s">
         <v>113</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -5397,7 +5382,7 @@
       <c r="E18" s="8">
         <v>500</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="6" t="s">
         <v>827</v>
       </c>
     </row>
@@ -5452,7 +5437,7 @@
       <c r="E21" s="8">
         <v>500</v>
       </c>
-      <c r="F21" s="40" t="s">
+      <c r="F21" s="6" t="s">
         <v>348</v>
       </c>
       <c r="G21" s="17"/>
@@ -5481,7 +5466,7 @@
       <c r="A23" s="8">
         <v>22</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="38" t="s">
         <v>346</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -5533,7 +5518,7 @@
       <c r="A26" s="10">
         <v>1</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="39" t="s">
         <v>134</v>
       </c>
       <c r="C26" s="9" t="s">
@@ -5573,7 +5558,7 @@
       <c r="A28" s="10">
         <v>3</v>
       </c>
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="37" t="s">
         <v>138</v>
       </c>
       <c r="C28" s="9" t="s">
@@ -5667,7 +5652,7 @@
       <c r="A33" s="10">
         <v>8</v>
       </c>
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="37" t="s">
         <v>146</v>
       </c>
       <c r="C33" s="9" t="s">
@@ -5704,7 +5689,7 @@
       <c r="A35" s="10">
         <v>10</v>
       </c>
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="38" t="s">
         <v>317</v>
       </c>
       <c r="C35" s="19" t="s">
@@ -5722,7 +5707,7 @@
       <c r="A36" s="10">
         <v>11</v>
       </c>
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="38" t="s">
         <v>318</v>
       </c>
       <c r="C36" s="19" t="s">
@@ -5740,7 +5725,7 @@
       <c r="A37" s="10">
         <v>12</v>
       </c>
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="38" t="s">
         <v>319</v>
       </c>
       <c r="C37" s="19" t="s">
@@ -5810,7 +5795,7 @@
       <c r="A41" s="10">
         <v>16</v>
       </c>
-      <c r="B41" s="39" t="s">
+      <c r="B41" s="37" t="s">
         <v>150</v>
       </c>
       <c r="C41" s="28" t="s">

</xml_diff>

<commit_message>
0109 protocol bug fix
</commit_message>
<xml_diff>
--- a/Mahtris 108/Assets/Document/Mahtris 108.xlsx
+++ b/Mahtris 108/Assets/Document/Mahtris 108.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dabbido\Desktop\Game Dev\GitHub\Mahtris-108\Mahtris 108\Assets\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28D8D52-A72F-43F0-B5BA-A9DBC53542D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A316BCA9-608D-40A5-B440-B5FDC26279FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="常规" sheetId="4" r:id="rId1"/>
@@ -1814,10 +1814,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>每轮游戏开始时，胡牌基础分+70，之后每秒-1（最低为1），胡牌后重置</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>每轮游戏开始时，胡牌&lt;color=#3296DC&gt;基础分+70&lt;/color&gt;，之后&lt;color=#3296DC&gt;每秒-1&lt;/color&gt;（最低为1），胡牌后重置</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -3079,6 +3075,10 @@
   <si>
     <t>Eraser</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>每轮游戏开始时，胡牌基础分+60，之后每秒-1（最低为1），胡牌后重置</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3181,7 +3181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3218,6 +3218,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3233,7 +3239,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3346,13 +3352,25 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3805,7 +3823,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -4192,16 +4210,16 @@
         <v>58</v>
       </c>
       <c r="E42" s="6" t="s">
+        <v>812</v>
+      </c>
+      <c r="F42" s="6" t="s">
         <v>813</v>
       </c>
-      <c r="F42" s="6" t="s">
-        <v>814</v>
-      </c>
       <c r="G42" s="6" t="s">
+        <v>812</v>
+      </c>
+      <c r="H42" s="6" t="s">
         <v>813</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.15">
@@ -5026,8 +5044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -5067,7 +5085,7 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="8" t="s">
         <v>101</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -5088,7 +5106,7 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="8" t="s">
         <v>103</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -5108,7 +5126,7 @@
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="18" t="s">
         <v>336</v>
       </c>
       <c r="C4" s="19" t="s">
@@ -5126,7 +5144,7 @@
       <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="8" t="s">
         <v>105</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -5143,7 +5161,7 @@
       <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="8" t="s">
         <v>107</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -5163,7 +5181,7 @@
       <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="8" t="s">
         <v>109</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -5184,7 +5202,7 @@
       <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="8" t="s">
         <v>111</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -5201,7 +5219,7 @@
       <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="8" t="s">
         <v>113</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -5214,14 +5232,14 @@
         <v>500</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="18" t="s">
         <v>341</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -5239,7 +5257,7 @@
       <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="8" t="s">
         <v>119</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -5259,11 +5277,11 @@
       <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="37" t="s">
-        <v>823</v>
+      <c r="B12" s="8" t="s">
+        <v>822</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D12" s="8">
         <v>1</v>
@@ -5272,18 +5290,18 @@
         <v>500</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="8">
         <v>12</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="8" t="s">
         <v>123</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E13" s="8">
         <v>500</v>
@@ -5296,7 +5314,7 @@
       <c r="A14" s="8">
         <v>13</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="8" t="s">
         <v>128</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -5316,7 +5334,7 @@
       <c r="A15" s="8">
         <v>14</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="8" t="s">
         <v>121</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -5333,7 +5351,7 @@
       <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="8" t="s">
         <v>116</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -5353,7 +5371,7 @@
       <c r="A17" s="8">
         <v>16</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="18" t="s">
         <v>261</v>
       </c>
       <c r="C17" s="19" t="s">
@@ -5373,7 +5391,7 @@
       <c r="A18" s="8">
         <v>17</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="8" t="s">
         <v>130</v>
       </c>
       <c r="C18" s="9" t="s">
@@ -5383,14 +5401,14 @@
         <v>500</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="8">
         <v>18</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="18" t="s">
         <v>259</v>
       </c>
       <c r="C19" s="19" t="s">
@@ -5408,7 +5426,7 @@
       <c r="A20" s="8">
         <v>19</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="18" t="s">
         <v>314</v>
       </c>
       <c r="C20" s="19" t="s">
@@ -5428,7 +5446,7 @@
       <c r="A21" s="8">
         <v>20</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="8" t="s">
         <v>132</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -5446,7 +5464,7 @@
       <c r="A22" s="8">
         <v>21</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="8" t="s">
         <v>124</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -5459,14 +5477,14 @@
         <v>500</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" s="8">
         <v>22</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="18" t="s">
         <v>346</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -5483,7 +5501,7 @@
       <c r="A24" s="8">
         <v>23</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="18" t="s">
         <v>502</v>
       </c>
       <c r="C24" s="19" t="s">
@@ -5501,7 +5519,7 @@
       <c r="A25" s="8">
         <v>24</v>
       </c>
-      <c r="B25" s="38" t="s">
+      <c r="B25" s="18" t="s">
         <v>251</v>
       </c>
       <c r="C25" s="28" t="s">
@@ -5518,7 +5536,7 @@
       <c r="A26" s="10">
         <v>1</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="1" t="s">
         <v>134</v>
       </c>
       <c r="C26" s="9" t="s">
@@ -5531,14 +5549,14 @@
         <v>500</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A27" s="10">
         <v>2</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="8" t="s">
         <v>136</v>
       </c>
       <c r="C27" s="9" t="s">
@@ -5558,7 +5576,7 @@
       <c r="A28" s="10">
         <v>3</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="8" t="s">
         <v>138</v>
       </c>
       <c r="C28" s="9" t="s">
@@ -5578,7 +5596,7 @@
       <c r="A29" s="10">
         <v>4</v>
       </c>
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="8" t="s">
         <v>140</v>
       </c>
       <c r="C29" s="9" t="s">
@@ -5595,7 +5613,7 @@
       <c r="A30" s="10">
         <v>5</v>
       </c>
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="18" t="s">
         <v>222</v>
       </c>
       <c r="C30" s="9" t="s">
@@ -5605,14 +5623,14 @@
         <v>2000</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" s="10">
         <v>6</v>
       </c>
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="8" t="s">
         <v>143</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -5632,7 +5650,7 @@
       <c r="A32" s="10">
         <v>7</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="18" t="s">
         <v>223</v>
       </c>
       <c r="C32" s="9" t="s">
@@ -5652,7 +5670,7 @@
       <c r="A33" s="10">
         <v>8</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="8" t="s">
         <v>146</v>
       </c>
       <c r="C33" s="9" t="s">
@@ -5669,7 +5687,7 @@
       <c r="A34" s="10">
         <v>9</v>
       </c>
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="18" t="s">
         <v>253</v>
       </c>
       <c r="C34" s="19" t="s">
@@ -5689,7 +5707,7 @@
       <c r="A35" s="10">
         <v>10</v>
       </c>
-      <c r="B35" s="38" t="s">
+      <c r="B35" s="18" t="s">
         <v>317</v>
       </c>
       <c r="C35" s="19" t="s">
@@ -5707,7 +5725,7 @@
       <c r="A36" s="10">
         <v>11</v>
       </c>
-      <c r="B36" s="38" t="s">
+      <c r="B36" s="18" t="s">
         <v>318</v>
       </c>
       <c r="C36" s="19" t="s">
@@ -5725,7 +5743,7 @@
       <c r="A37" s="10">
         <v>12</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="18" t="s">
         <v>319</v>
       </c>
       <c r="C37" s="19" t="s">
@@ -5743,7 +5761,7 @@
       <c r="A38" s="10">
         <v>13</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="8" t="s">
         <v>148</v>
       </c>
       <c r="C38" s="9" t="s">
@@ -5760,11 +5778,11 @@
       <c r="A39" s="10">
         <v>14</v>
       </c>
-      <c r="B39" s="37" t="s">
+      <c r="B39" s="8" t="s">
+        <v>820</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>821</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>822</v>
       </c>
       <c r="E39" s="8">
         <v>3000</v>
@@ -5777,7 +5795,7 @@
       <c r="A40" s="10">
         <v>15</v>
       </c>
-      <c r="B40" s="38" t="s">
+      <c r="B40" s="18" t="s">
         <v>323</v>
       </c>
       <c r="C40" s="29" t="s">
@@ -5795,7 +5813,7 @@
       <c r="A41" s="10">
         <v>16</v>
       </c>
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="8" t="s">
         <v>150</v>
       </c>
       <c r="C41" s="28" t="s">
@@ -6093,8 +6111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N172"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" activeCellId="2" sqref="E14:E15 E19:E20 E25:E41"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -6138,7 +6156,7 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="37" t="s">
         <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -6154,7 +6172,7 @@
         <v>379</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="M2" s="17"/>
     </row>
@@ -6162,7 +6180,7 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="42" t="s">
         <v>226</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -6174,18 +6192,18 @@
       <c r="E3" s="8">
         <v>5000</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="G3" s="17" t="s">
         <v>510</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="41" t="s">
         <v>232</v>
       </c>
       <c r="C4" s="18" t="s">
@@ -6197,18 +6215,18 @@
       <c r="E4" s="8">
         <v>5000</v>
       </c>
-      <c r="F4" s="17" t="s">
-        <v>516</v>
+      <c r="F4" s="6" t="s">
+        <v>515</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="37" t="s">
         <v>166</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -6231,7 +6249,7 @@
       <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="42" t="s">
         <v>225</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -6243,7 +6261,7 @@
       <c r="E6" s="8">
         <v>5000</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="6" t="s">
         <v>364</v>
       </c>
       <c r="G6" s="17" t="s">
@@ -6254,7 +6272,7 @@
       <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="37" t="s">
         <v>173</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -6267,17 +6285,17 @@
         <v>5000</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="37" t="s">
         <v>179</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -6300,7 +6318,7 @@
       <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="37" t="s">
         <v>171</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -6312,18 +6330,18 @@
       <c r="E9" s="8">
         <v>5000</v>
       </c>
-      <c r="F9" s="17" t="s">
-        <v>520</v>
+      <c r="F9" s="6" t="s">
+        <v>519</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="37" t="s">
         <v>156</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -6347,7 +6365,7 @@
       <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="40" t="s">
         <v>158</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -6370,7 +6388,7 @@
       <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="41" t="s">
         <v>327</v>
       </c>
       <c r="C12" s="30" t="s">
@@ -6386,14 +6404,14 @@
         <v>328</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" s="8">
         <v>12</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="41" t="s">
         <v>389</v>
       </c>
       <c r="C13" s="30" t="s">
@@ -6409,14 +6427,14 @@
         <v>388</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14" s="8">
         <v>13</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="41" t="s">
         <v>329</v>
       </c>
       <c r="C14" s="30" t="s">
@@ -6429,14 +6447,14 @@
         <v>331</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15" s="8">
         <v>14</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="37" t="s">
         <v>164</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -6456,7 +6474,7 @@
       <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="37" t="s">
         <v>162</v>
       </c>
       <c r="C16" s="18" t="s">
@@ -6472,7 +6490,7 @@
         <v>282</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H16" s="17"/>
     </row>
@@ -6480,7 +6498,7 @@
       <c r="A17" s="8">
         <v>16</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="42" t="s">
         <v>258</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -6492,7 +6510,7 @@
       <c r="E17" s="8">
         <v>5000</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="6" t="s">
         <v>368</v>
       </c>
       <c r="G17" s="17" t="s">
@@ -6503,7 +6521,7 @@
       <c r="A18" s="8">
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="40" t="s">
         <v>186</v>
       </c>
       <c r="C18" s="30" t="s">
@@ -6519,14 +6537,14 @@
         <v>354</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19" s="8">
         <v>18</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="42" t="s">
         <v>254</v>
       </c>
       <c r="C19" s="8" t="s">
@@ -6548,7 +6566,7 @@
       <c r="A20" s="8">
         <v>19</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="41" t="s">
         <v>227</v>
       </c>
       <c r="C20" s="30" t="s">
@@ -6568,7 +6586,7 @@
       <c r="A21" s="8">
         <v>20</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="41" t="s">
         <v>256</v>
       </c>
       <c r="C21" s="30" t="s">
@@ -6591,7 +6609,7 @@
       <c r="A22" s="8">
         <v>21</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="41" t="s">
         <v>231</v>
       </c>
       <c r="C22" s="18" t="s">
@@ -6614,7 +6632,7 @@
       <c r="A23" s="8">
         <v>22</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="41" t="s">
         <v>332</v>
       </c>
       <c r="C23" s="30" t="s">
@@ -6637,7 +6655,7 @@
       <c r="A24" s="8">
         <v>23</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="37" t="s">
         <v>181</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -6660,7 +6678,7 @@
       <c r="A25" s="8">
         <v>24</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="42" t="s">
         <v>224</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -6680,7 +6698,7 @@
       <c r="A26" s="8">
         <v>25</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="25" t="s">
         <v>233</v>
       </c>
       <c r="C26" s="18" t="s">
@@ -6700,7 +6718,7 @@
       <c r="A27" s="8">
         <v>26</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="41" t="s">
         <v>334</v>
       </c>
       <c r="C27" s="30" t="s">
@@ -6720,7 +6738,7 @@
       <c r="A28" s="8">
         <v>27</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="41" t="s">
         <v>228</v>
       </c>
       <c r="C28" s="30" t="s">
@@ -6740,7 +6758,7 @@
       <c r="A29" s="8">
         <v>28</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="37" t="s">
         <v>176</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -6760,7 +6778,7 @@
       <c r="A30" s="8">
         <v>29</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="41" t="s">
         <v>255</v>
       </c>
       <c r="C30" s="30" t="s">
@@ -6780,7 +6798,7 @@
       <c r="A31" s="8">
         <v>30</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="39" t="s">
         <v>163</v>
       </c>
       <c r="C31" s="8" t="s">
@@ -6800,7 +6818,7 @@
       <c r="A32" s="8">
         <v>31</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="37" t="s">
         <v>169</v>
       </c>
       <c r="C32" s="8" t="s">
@@ -6820,7 +6838,7 @@
       <c r="A33" s="8">
         <v>32</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="43" t="s">
         <v>304</v>
       </c>
       <c r="C33" s="18" t="s">
@@ -6840,7 +6858,7 @@
       <c r="A34" s="8">
         <v>33</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="41" t="s">
         <v>385</v>
       </c>
       <c r="C34" s="30" t="s">
@@ -6860,7 +6878,7 @@
       <c r="A35" s="8">
         <v>34</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="38" t="s">
         <v>234</v>
       </c>
       <c r="C35" s="30" t="s">
@@ -6880,7 +6898,7 @@
       <c r="A36" s="8">
         <v>35</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="25" t="s">
         <v>245</v>
       </c>
       <c r="C36" s="18" t="s">
@@ -6900,7 +6918,7 @@
       <c r="A37" s="8">
         <v>36</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="41" t="s">
         <v>335</v>
       </c>
       <c r="C37" s="30" t="s">
@@ -6920,7 +6938,7 @@
       <c r="A38" s="8">
         <v>37</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="41" t="s">
         <v>325</v>
       </c>
       <c r="C38" s="30" t="s">
@@ -6933,14 +6951,14 @@
         <v>330</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="8">
         <v>38</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="41" t="s">
         <v>257</v>
       </c>
       <c r="C39" s="34" t="s">
@@ -6960,7 +6978,7 @@
       <c r="A40" s="8">
         <v>39</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="41" t="s">
         <v>229</v>
       </c>
       <c r="C40" s="35" t="s">
@@ -6980,7 +6998,7 @@
       <c r="A41" s="8">
         <v>40</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="37" t="s">
         <v>184</v>
       </c>
       <c r="C41" s="27" t="s">
@@ -7804,7 +7822,7 @@
         <v>60</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>44</v>
@@ -8034,7 +8052,7 @@
         <v>414</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
@@ -8987,32 +9005,32 @@
     </row>
     <row r="22" spans="1:3" ht="90.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="22" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="90.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="22" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="90.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="22" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="90.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="22" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="90.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="22" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="90.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="22" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
   </sheetData>
@@ -9040,126 +9058,126 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="17" t="s">
+        <v>524</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>525</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="17" t="s">
         <v>526</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>527</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>528</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>529</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>530</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="D2" s="17" t="s">
         <v>531</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="17" t="s">
         <v>532</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>533</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>534</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="D3" s="17" t="s">
         <v>535</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>536</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>541</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="D4" s="17" t="s">
         <v>542</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>543</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C5" s="17" t="s">
+        <v>674</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>675</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="E5" s="17" t="s">
         <v>676</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D6" s="17" t="s">
+        <v>677</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>678</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>553</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>553</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>554</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>554</v>
-      </c>
-      <c r="D7" s="17" t="s">
+      <c r="E7" s="17" t="s">
         <v>555</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>48</v>
@@ -9168,66 +9186,66 @@
         <v>48</v>
       </c>
       <c r="D8" s="17" t="s">
+        <v>544</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>545</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>546</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>547</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="D9" s="17" t="s">
         <v>548</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="E9" s="17" t="s">
         <v>549</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="17" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>551</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="E10" s="17" t="s">
         <v>552</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="17" t="s">
+        <v>537</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>538</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="E11" s="17" t="s">
         <v>539</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>48</v>
@@ -9236,1064 +9254,1064 @@
         <v>48</v>
       </c>
       <c r="D12" s="17" t="s">
+        <v>544</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>545</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B13" s="17" t="s">
+        <v>546</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>547</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="D13" s="17" t="s">
         <v>548</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="E13" s="17" t="s">
         <v>549</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>551</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="E14" s="17" t="s">
         <v>552</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
+        <v>574</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>575</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>576</v>
-      </c>
       <c r="C15" s="17" t="s">
+        <v>679</v>
+      </c>
+      <c r="D15" s="17" t="s">
         <v>680</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="E15" s="17" t="s">
         <v>681</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>577</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>578</v>
-      </c>
       <c r="C16" s="17" t="s">
+        <v>682</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>683</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="E16" s="17" t="s">
         <v>684</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="17" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D18" s="17" t="s">
+        <v>686</v>
+      </c>
+      <c r="E18" s="17" t="s">
         <v>687</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C19" s="17" t="s">
+        <v>688</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>689</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="E19" s="17" t="s">
         <v>690</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="17" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C20" s="17" t="s">
+        <v>691</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>692</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="E20" s="17" t="s">
         <v>693</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="17" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C21" s="17" t="s">
+        <v>694</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>695</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="E21" s="17" t="s">
         <v>696</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="17" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C22" s="17" t="s">
+        <v>697</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>698</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="E22" s="17" t="s">
         <v>699</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="17" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C23" s="17" t="s">
+        <v>700</v>
+      </c>
+      <c r="D23" s="17" t="s">
         <v>701</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="E23" s="17" t="s">
         <v>702</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="17" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C24" s="17" t="s">
+        <v>703</v>
+      </c>
+      <c r="D24" s="17" t="s">
         <v>704</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="E24" s="17" t="s">
         <v>705</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A25" s="17" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C25" s="17" t="s">
+        <v>674</v>
+      </c>
+      <c r="D25" s="17" t="s">
         <v>675</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="E25" s="17" t="s">
         <v>676</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="17" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D26" s="17" t="s">
+        <v>686</v>
+      </c>
+      <c r="E26" s="17" t="s">
         <v>687</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="17" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C27" s="17" t="s">
+        <v>688</v>
+      </c>
+      <c r="D27" s="17" t="s">
         <v>689</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="E27" s="17" t="s">
         <v>690</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="17" t="s">
+        <v>806</v>
+      </c>
+      <c r="B28" s="17" t="s">
         <v>807</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="C28" s="17" t="s">
         <v>808</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>809</v>
-      </c>
       <c r="D28" s="17" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="17" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D29" s="17" t="s">
+        <v>677</v>
+      </c>
+      <c r="E29" s="17" t="s">
         <v>678</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="17" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C30" s="17" t="s">
+        <v>706</v>
+      </c>
+      <c r="D30" s="17" t="s">
         <v>707</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="E30" s="17" t="s">
         <v>708</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="B31" s="17" t="s">
         <v>602</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>603</v>
-      </c>
       <c r="C31" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="D31" s="17" t="s">
         <v>710</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="E31" s="17" t="s">
         <v>711</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="17" t="s">
+        <v>603</v>
+      </c>
+      <c r="B32" s="17" t="s">
         <v>604</v>
       </c>
-      <c r="B32" s="17" t="s">
-        <v>605</v>
-      </c>
       <c r="C32" s="17" t="s">
+        <v>712</v>
+      </c>
+      <c r="D32" s="17" t="s">
         <v>713</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="E32" s="17" t="s">
         <v>714</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="B33" s="17" t="s">
         <v>606</v>
       </c>
-      <c r="B33" s="17" t="s">
-        <v>607</v>
-      </c>
       <c r="C33" s="17" t="s">
+        <v>715</v>
+      </c>
+      <c r="D33" s="17" t="s">
         <v>716</v>
       </c>
-      <c r="D33" s="17" t="s">
-        <v>717</v>
-      </c>
       <c r="E33" s="17" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="17" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C34" s="17" t="s">
+        <v>717</v>
+      </c>
+      <c r="D34" s="17" t="s">
         <v>718</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="E34" s="17" t="s">
         <v>719</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="17" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D35" s="17" t="s">
+        <v>720</v>
+      </c>
+      <c r="E35" s="17" t="s">
         <v>721</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="17" t="s">
+        <v>611</v>
+      </c>
+      <c r="B36" s="17" t="s">
         <v>612</v>
       </c>
-      <c r="B36" s="17" t="s">
-        <v>613</v>
-      </c>
       <c r="C36" s="17" t="s">
+        <v>722</v>
+      </c>
+      <c r="D36" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="E36" s="17" t="s">
         <v>724</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="17" t="s">
+        <v>613</v>
+      </c>
+      <c r="B37" s="17" t="s">
         <v>614</v>
       </c>
-      <c r="B37" s="17" t="s">
-        <v>615</v>
-      </c>
       <c r="C37" s="17" t="s">
+        <v>725</v>
+      </c>
+      <c r="D37" s="17" t="s">
         <v>726</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="E37" s="17" t="s">
         <v>727</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="17" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C38" s="17" t="s">
+        <v>728</v>
+      </c>
+      <c r="D38" s="17" t="s">
         <v>729</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="E38" s="17" t="s">
         <v>730</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="17" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C39" s="17" t="s">
+        <v>731</v>
+      </c>
+      <c r="D39" s="17" t="s">
         <v>732</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="E39" s="17" t="s">
         <v>733</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="17" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C40" s="17" t="s">
+        <v>734</v>
+      </c>
+      <c r="D40" s="17" t="s">
         <v>735</v>
       </c>
-      <c r="D40" s="17" t="s">
-        <v>736</v>
-      </c>
       <c r="E40" s="17" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" s="17" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C41" s="17" t="s">
+        <v>736</v>
+      </c>
+      <c r="D41" s="17" t="s">
         <v>737</v>
       </c>
-      <c r="D41" s="17" t="s">
+      <c r="E41" s="17" t="s">
         <v>738</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="17" t="s">
+        <v>627</v>
+      </c>
+      <c r="B42" s="17" t="s">
         <v>628</v>
       </c>
-      <c r="B42" s="17" t="s">
-        <v>629</v>
-      </c>
       <c r="C42" s="17" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D42" s="17" t="s">
+        <v>739</v>
+      </c>
+      <c r="E42" s="17" t="s">
         <v>740</v>
-      </c>
-      <c r="E42" s="17" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" s="17" t="s">
+        <v>629</v>
+      </c>
+      <c r="B43" s="17" t="s">
         <v>630</v>
       </c>
-      <c r="B43" s="17" t="s">
-        <v>631</v>
-      </c>
       <c r="C43" s="17" t="s">
+        <v>741</v>
+      </c>
+      <c r="D43" s="17" t="s">
         <v>742</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="E43" s="17" t="s">
         <v>743</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" s="17" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C44" s="17" t="s">
+        <v>744</v>
+      </c>
+      <c r="D44" s="17" t="s">
         <v>745</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="E44" s="36" t="s">
         <v>746</v>
-      </c>
-      <c r="E44" s="36" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" s="17" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C45" s="17" t="s">
+        <v>747</v>
+      </c>
+      <c r="D45" s="17" t="s">
         <v>748</v>
       </c>
-      <c r="D45" s="17" t="s">
+      <c r="E45" s="17" t="s">
         <v>749</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>750</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" s="17" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C46" s="17" t="s">
+        <v>750</v>
+      </c>
+      <c r="D46" s="17" t="s">
         <v>751</v>
       </c>
-      <c r="D46" s="17" t="s">
+      <c r="E46" s="17" t="s">
         <v>752</v>
-      </c>
-      <c r="E46" s="17" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="17" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C47" s="17" t="s">
+        <v>753</v>
+      </c>
+      <c r="D47" s="17" t="s">
         <v>754</v>
       </c>
-      <c r="D47" s="17" t="s">
+      <c r="E47" s="17" t="s">
         <v>755</v>
-      </c>
-      <c r="E47" s="17" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C48" s="17" t="s">
+        <v>756</v>
+      </c>
+      <c r="D48" s="17" t="s">
         <v>757</v>
       </c>
-      <c r="D48" s="17" t="s">
-        <v>758</v>
-      </c>
       <c r="E48" s="17" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="17" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C49" s="17" t="s">
+        <v>758</v>
+      </c>
+      <c r="D49" s="17" t="s">
         <v>759</v>
       </c>
-      <c r="D49" s="17" t="s">
+      <c r="E49" s="17" t="s">
         <v>760</v>
-      </c>
-      <c r="E49" s="17" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" s="17" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C50" s="17" t="s">
+        <v>761</v>
+      </c>
+      <c r="D50" s="17" t="s">
         <v>762</v>
       </c>
-      <c r="D50" s="17" t="s">
+      <c r="E50" s="17" t="s">
         <v>763</v>
-      </c>
-      <c r="E50" s="17" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="17" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C51" s="17" t="s">
+        <v>688</v>
+      </c>
+      <c r="D51" s="17" t="s">
         <v>689</v>
       </c>
-      <c r="D51" s="17" t="s">
+      <c r="E51" s="17" t="s">
         <v>690</v>
-      </c>
-      <c r="E51" s="17" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52" s="17" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D52" s="17" t="s">
+        <v>686</v>
+      </c>
+      <c r="E52" s="17" t="s">
         <v>687</v>
-      </c>
-      <c r="E52" s="17" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A53" s="17" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C53" s="17" t="s">
+        <v>764</v>
+      </c>
+      <c r="D53" s="17" t="s">
         <v>765</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="E53" s="17" t="s">
         <v>766</v>
-      </c>
-      <c r="E53" s="17" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A54" s="17" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C54" s="17" t="s">
+        <v>758</v>
+      </c>
+      <c r="D54" s="17" t="s">
         <v>759</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="E54" s="17" t="s">
         <v>760</v>
-      </c>
-      <c r="E54" s="17" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A55" s="17" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E55" s="17" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A56" s="17" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E56" s="17" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A57" s="17" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E57" s="17" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A58" s="17" t="s">
+        <v>656</v>
+      </c>
+      <c r="B58" s="17" t="s">
         <v>657</v>
       </c>
-      <c r="B58" s="17" t="s">
-        <v>658</v>
-      </c>
       <c r="C58" s="17" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D58" s="17" t="s">
+        <v>775</v>
+      </c>
+      <c r="E58" s="17" t="s">
         <v>776</v>
-      </c>
-      <c r="E58" s="17" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A59" s="17" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C59" s="17" t="s">
+        <v>777</v>
+      </c>
+      <c r="D59" s="17" t="s">
         <v>778</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="E59" s="17" t="s">
         <v>779</v>
-      </c>
-      <c r="E59" s="17" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A60" s="17" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D60" s="17" t="s">
+        <v>780</v>
+      </c>
+      <c r="E60" s="17" t="s">
         <v>781</v>
-      </c>
-      <c r="E60" s="17" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" s="17" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C61" s="17" t="s">
+        <v>782</v>
+      </c>
+      <c r="D61" s="17" t="s">
         <v>783</v>
       </c>
-      <c r="D61" s="17" t="s">
+      <c r="E61" s="17" t="s">
         <v>784</v>
-      </c>
-      <c r="E61" s="17" t="s">
-        <v>785</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A62" s="17" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C62" s="17" t="s">
+        <v>741</v>
+      </c>
+      <c r="D62" s="17" t="s">
         <v>742</v>
       </c>
-      <c r="D62" s="17" t="s">
+      <c r="E62" s="17" t="s">
         <v>743</v>
-      </c>
-      <c r="E62" s="17" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A63" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="B63" s="17" t="s">
         <v>664</v>
       </c>
-      <c r="B63" s="17" t="s">
-        <v>665</v>
-      </c>
       <c r="C63" s="17" t="s">
+        <v>785</v>
+      </c>
+      <c r="D63" s="17" t="s">
         <v>786</v>
       </c>
-      <c r="D63" s="17" t="s">
+      <c r="E63" s="17" t="s">
         <v>787</v>
-      </c>
-      <c r="E63" s="17" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A64" s="17" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C64" s="17" t="s">
+        <v>790</v>
+      </c>
+      <c r="D64" s="17" t="s">
         <v>791</v>
       </c>
-      <c r="D64" s="17" t="s">
+      <c r="E64" s="17" t="s">
         <v>792</v>
-      </c>
-      <c r="E64" s="17" t="s">
-        <v>793</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A65" s="17" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C65" s="17" t="s">
+        <v>793</v>
+      </c>
+      <c r="D65" s="17" t="s">
         <v>794</v>
       </c>
-      <c r="D65" s="17" t="s">
+      <c r="E65" s="17" t="s">
         <v>795</v>
-      </c>
-      <c r="E65" s="17" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A66" s="17" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D66" s="17" t="s">
+        <v>686</v>
+      </c>
+      <c r="E66" s="17" t="s">
         <v>687</v>
-      </c>
-      <c r="E66" s="17" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A67" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C67" s="17" t="s">
+        <v>796</v>
+      </c>
+      <c r="D67" s="17" t="s">
         <v>797</v>
       </c>
-      <c r="D67" s="17" t="s">
+      <c r="E67" s="17" t="s">
         <v>798</v>
-      </c>
-      <c r="E67" s="17" t="s">
-        <v>799</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A68" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C68" s="17" t="s">
+        <v>688</v>
+      </c>
+      <c r="D68" s="17" t="s">
         <v>689</v>
       </c>
-      <c r="D68" s="17" t="s">
+      <c r="E68" s="17" t="s">
         <v>690</v>
-      </c>
-      <c r="E68" s="17" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A69" s="17" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C69" s="17" t="s">
+        <v>799</v>
+      </c>
+      <c r="D69" s="17" t="s">
         <v>800</v>
       </c>
-      <c r="D69" s="17" t="s">
+      <c r="E69" s="17" t="s">
         <v>801</v>
-      </c>
-      <c r="E69" s="17" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A70" s="17" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D70" s="17" t="s">
+        <v>686</v>
+      </c>
+      <c r="E70" s="17" t="s">
         <v>687</v>
-      </c>
-      <c r="E70" s="17" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A71" s="17" t="s">
+        <v>624</v>
+      </c>
+      <c r="B71" s="17" t="s">
         <v>625</v>
       </c>
-      <c r="B71" s="17" t="s">
-        <v>626</v>
-      </c>
       <c r="C71" s="17" t="s">
+        <v>796</v>
+      </c>
+      <c r="D71" s="17" t="s">
         <v>797</v>
       </c>
-      <c r="D71" s="17" t="s">
-        <v>798</v>
-      </c>
       <c r="E71" s="17" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A72" s="17" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C72" s="17" t="s">
+        <v>688</v>
+      </c>
+      <c r="D72" s="17" t="s">
         <v>689</v>
       </c>
-      <c r="D72" s="17" t="s">
+      <c r="E72" s="17" t="s">
         <v>690</v>
-      </c>
-      <c r="E72" s="17" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A73" s="17" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B73" s="17" t="s">
         <v>113</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D73" s="17" t="s">
         <v>114</v>
       </c>
       <c r="E73" s="17" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A74" s="17" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B74" s="17" t="s">
         <v>115</v>
       </c>
       <c r="C74" s="17" t="s">
+        <v>803</v>
+      </c>
+      <c r="D74" s="17" t="s">
+        <v>805</v>
+      </c>
+      <c r="E74" s="17" t="s">
         <v>804</v>
-      </c>
-      <c r="D74" s="17" t="s">
-        <v>806</v>
-      </c>
-      <c r="E74" s="17" t="s">
-        <v>805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>